<commit_message>
fix: event_settings.xlsx is updated for previous commit
</commit_message>
<xml_diff>
--- a/data/event_settings.xlsx
+++ b/data/event_settings.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\79778\Desktop\streamlit_orchestrator\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\79778\AppData\Local\Temp\Rar$DIa25100.30090\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{225C2677-9C3F-4145-BF03-88E3BAF891CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4066FF1-AF21-4DAD-A709-5F1D49042653}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -96,13 +96,13 @@
     <t>Запуск скважин</t>
   </si>
   <si>
-    <t>{"adap_period": ["boundary_code", "permeability", "skin", "res_width",  "res_length", "length_hor_well_bore", "length_half_fracture", "number_fractures"], "test_period": []}</t>
-  </si>
-  <si>
     <t>{"adap_period": ["skin", "boundary_code"], "test_period": []}</t>
   </si>
   <si>
     <t>{"adap_period": ["kind_code", "boundary_code",  "skin", "length_half_fracture", "number_fractures"], "test_period": []}</t>
+  </si>
+  <si>
+    <t>{"adap_period": ["boundary_code", "permeability", "skin", "res_radius", "length_hor_well_bore", "length_half_fracture", "number_fractures"], "test_period": []}</t>
   </si>
 </sst>
 </file>
@@ -423,13 +423,13 @@
   <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="52.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="155.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="133.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
@@ -445,7 +445,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -453,7 +453,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -461,7 +461,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -469,7 +469,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -477,7 +477,7 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -485,7 +485,7 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -493,7 +493,7 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -501,7 +501,7 @@
         <v>22</v>
       </c>
       <c r="B9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
@@ -509,7 +509,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -517,7 +517,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
@@ -525,7 +525,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
@@ -533,7 +533,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
@@ -541,7 +541,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
@@ -549,7 +549,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
@@ -557,7 +557,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
@@ -565,7 +565,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
@@ -573,7 +573,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
@@ -581,7 +581,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
@@ -589,7 +589,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
@@ -597,7 +597,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
@@ -605,7 +605,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>